<commit_message>
Update VLOOKUP lecture Excel file
Revised 07_VLOOKUP.xlsx with new or corrected data, formulas, or formatting for the MCfCL-07 lecture. See file for specific changes.
</commit_message>
<xml_diff>
--- a/MCfCL-07-Lecture/07_VLOOKUP.xlsx
+++ b/MCfCL-07-Lecture/07_VLOOKUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tetsu\github\2025-SIT-MCfCL\MCfCL-07-Lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5610EA-AB07-4C11-9E8C-2CF7C2CDCEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB8D69-1EC4-4CED-8E32-35CB2034A0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="6150" windowWidth="21480" windowHeight="12015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="5835" windowWidth="26925" windowHeight="18345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="商品マスタ" sheetId="1" r:id="rId1"/>
@@ -501,9 +501,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="177" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -664,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -694,9 +693,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -748,13 +744,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,16 +1070,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1091,10 +1087,10 @@
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="4">
@@ -1105,10 +1101,10 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="4">
@@ -1119,10 +1115,10 @@
       <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="4">
@@ -1133,10 +1129,10 @@
       <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="5">
@@ -1147,10 +1143,10 @@
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="25" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="5">
@@ -1161,10 +1157,10 @@
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="4">
@@ -1175,10 +1171,10 @@
       <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="25" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="5">
@@ -1189,10 +1185,10 @@
       <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="25" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="4">
@@ -1203,10 +1199,10 @@
       <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="4">
@@ -1217,10 +1213,10 @@
       <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="4">
@@ -1231,10 +1227,10 @@
       <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="4">
@@ -1245,10 +1241,10 @@
       <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="5">
@@ -1259,10 +1255,10 @@
       <c r="C15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="4">
@@ -1273,10 +1269,10 @@
       <c r="C16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>38</v>
       </c>
       <c r="F16" s="4">
@@ -1287,10 +1283,10 @@
       <c r="C17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="4">
@@ -1301,10 +1297,10 @@
       <c r="C18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>57</v>
       </c>
       <c r="F18" s="4">
@@ -1315,10 +1311,10 @@
       <c r="C19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="27" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="4">
@@ -1329,10 +1325,10 @@
       <c r="C20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="5">
@@ -1343,10 +1339,10 @@
       <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="4">
@@ -1357,10 +1353,10 @@
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>44</v>
       </c>
       <c r="F22" s="4">
@@ -1383,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D3:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1443,8 +1439,8 @@
       <c r="I4" s="9">
         <v>7</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="4:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1462,8 +1458,8 @@
       <c r="I5" s="9">
         <v>2</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="4:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1481,8 +1477,10 @@
       <c r="I6" s="9">
         <v>5</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="29"/>
+      <c r="J6" s="29">
+        <v>1000</v>
+      </c>
+      <c r="K6" s="30"/>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="4:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1500,8 +1498,8 @@
       <c r="I7" s="9">
         <v>8</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="4:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -1519,7 +1517,7 @@
       <c r="I8" s="9">
         <v>4</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="29"/>
       <c r="K8" s="30"/>
       <c r="L8" s="8" t="s">
         <v>7</v>
@@ -1558,13 +1556,13 @@
       </c>
     </row>
     <row r="6" spans="6:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>59</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1572,13 +1570,13 @@
       </c>
     </row>
     <row r="7" spans="6:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>60</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>69</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1586,13 +1584,13 @@
       </c>
     </row>
     <row r="8" spans="6:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>70</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>79</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1600,13 +1598,13 @@
       </c>
     </row>
     <row r="9" spans="6:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>80</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>89</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1614,13 +1612,13 @@
       </c>
     </row>
     <row r="10" spans="6:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>90</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>100</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1637,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1650,597 +1648,597 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>78</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>82</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="15">
         <v>71</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="20"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>85</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>70</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="15">
         <v>80</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="20"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>69</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>90</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <v>85</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="20"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>91</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>79</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <v>88</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="20"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>58</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>64</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>60</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="20"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>89</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>96</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <v>92</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>74</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>83</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <v>76</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="20"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>66</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <v>75</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <v>70</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="20"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>93</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>88</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="15">
         <v>90</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="20"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>81</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>69</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="15">
         <v>78</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="20"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>72</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>77</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="15">
         <v>65</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="20"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>86</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>91</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <v>84</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="20"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>61</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>68</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="15">
         <v>73</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="20"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>95</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>85</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <v>91</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="20"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>79</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>80</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="15">
         <v>82</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="20"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="14">
         <v>67</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>73</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="15">
         <v>69</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>88</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>93</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="15">
         <v>87</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="20"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="14">
         <v>70</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <v>62</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="15">
         <v>75</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="20"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="14">
         <v>83</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>86</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="15">
         <v>81</v>
       </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="20"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="14">
         <v>59</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="12">
         <v>71</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="15">
         <v>63</v>
       </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="20"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="14">
         <v>92</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <v>95</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="15">
         <v>89</v>
       </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="20"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="14">
         <v>76</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <v>84</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="15">
         <v>77</v>
       </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="20"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="14">
         <v>80</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <v>78</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="15">
         <v>83</v>
       </c>
-      <c r="G27" s="31"/>
-      <c r="H27" s="20"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="14">
         <v>64</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>67</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <v>68</v>
       </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="20"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="14">
         <v>87</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <v>89</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="15">
         <v>93</v>
       </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="20"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="14">
         <v>73</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>76</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="15">
         <v>66</v>
       </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="20"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="14">
         <v>90</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="12">
         <v>92</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="15">
         <v>86</v>
       </c>
-      <c r="G31" s="31"/>
-      <c r="H31" s="20"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="14">
         <v>68</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <v>74</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="15">
         <v>72</v>
       </c>
-      <c r="G32" s="31"/>
-      <c r="H32" s="20"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="19"/>
     </row>
     <row r="33" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="14">
         <v>84</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="12">
         <v>81</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="15">
         <v>79</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="20"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="14">
         <v>94</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="12">
         <v>87</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="15">
         <v>94</v>
       </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="20"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>